<commit_message>
Added bubble diagram for server temperature state machine
</commit_message>
<xml_diff>
--- a/questions/Server Command Table A8.xlsx
+++ b/questions/Server Command Table A8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhruv\SimplicityStudio\v5_workspace\ecen5823-assignment8-DhruvHMehta\questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D1D11F-23D4-4750-BF57-2B0AEE081FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC8AAB4-53CF-4353-8FEF-ED22D9249B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
   <si>
     <t>Event</t>
   </si>
@@ -242,12 +242,15 @@
   <si>
     <t>Confirms the request for bonding as per config flags</t>
   </si>
+  <si>
+    <t>Server Bubble Diagram</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -282,6 +285,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -322,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -360,6 +370,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -444,6 +457,1857 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>94622</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>137722</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1765169</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>125405</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Oval 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE2E046B-217F-4378-911B-24CBAD9D8A64}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4384682" y="12855502"/>
+          <a:ext cx="1670547" cy="1511683"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>IDLE</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>261668</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>42198</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2020804</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>106540</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Oval 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9066E4F7-2A45-4B28-9D16-A279BE401DF4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7020608" y="11045478"/>
+          <a:ext cx="1759136" cy="1588342"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>POWERUP</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1661380</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>89690</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1007827</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>77373</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Oval 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C9A4B51-6C98-40F9-A2A3-78744D32A879}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8420320" y="15664970"/>
+          <a:ext cx="1670547" cy="1511683"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>WAIT</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>679287</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>170554</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Oval 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D426B025-40D3-42EA-A4D1-A382DE216800}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9762327" y="12915900"/>
+          <a:ext cx="1675293" cy="1496434"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>MEASURE</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1168077</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>89690</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>369744</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>77373</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Oval 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{153051B7-0EE9-4ED9-B8B1-C3F6691DC9E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5458137" y="15664970"/>
+          <a:ext cx="1670547" cy="1511683"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>REPORT</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>929897</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>74369</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>261669</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>137722</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Connector: Curved 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D44A9940-4DAD-49FA-8D55-08190D24D8BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="17" idx="0"/>
+          <a:endCxn id="18" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="5612356" y="11447250"/>
+          <a:ext cx="1015853" cy="1800652"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2020804</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>74369</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1516934</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Connector: Curved 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4C0A771-F54E-4351-B752-D1684EACADC9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="18" idx="6"/>
+          <a:endCxn id="20" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8779744" y="11839649"/>
+          <a:ext cx="1820230" cy="1076251"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>172554</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>170554</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1516934</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>89690</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Connector: Curved 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D030CAF9-BA34-4796-9D84-A8FA8B374A82}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="20" idx="4"/>
+          <a:endCxn id="19" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="9301466" y="14366462"/>
+          <a:ext cx="1252636" cy="1344380"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>369744</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>83532</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1661380</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>96232</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Connector: Curved 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{206B1AB5-7ABE-4454-81CB-BDD28AE8AADB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="19" idx="2"/>
+          <a:endCxn id="21" idx="6"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="7128684" y="16420812"/>
+          <a:ext cx="1291636" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>929897</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>125405</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2003352</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>89690</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Connector: Curved 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0ADEBFAF-A0FF-48DA-9B1E-08ED10B336D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="21" idx="0"/>
+          <a:endCxn id="17" idx="4"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="5107792" y="14479350"/>
+          <a:ext cx="1297785" cy="1073455"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>756751</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>113140</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>663177</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>119426</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="TextBox 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{472EFE1B-6B51-42EE-A262-7C340BEA1F64}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5046811" y="11687920"/>
+          <a:ext cx="2375306" cy="387286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>If(Underflow)</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1000"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>powerOnSi7021()</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>899751</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>161539</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>950957</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>124801</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="TextBox 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE839498-E750-430A-8D42-D662F8964805}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9982791" y="14974819"/>
+          <a:ext cx="2375306" cy="534762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>If(I2C Complete)</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1000"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Remove EM1 requirement</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1000"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>waitConversionTimeSi7021()</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>679287</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>32870</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>730493</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>186632</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="TextBox 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07D3D09F-9BA9-474C-A0B7-4345B6D9D82D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9762327" y="11607650"/>
+          <a:ext cx="2375306" cy="534762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>If(Comp1)</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1000"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Add EM1 requirement</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1000"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>getTemperatureSi7021()</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>254048</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>101247</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>305254</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>64509</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="TextBox 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{411BD206-4CC8-4706-AD91-9F990AF71C39}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7012988" y="15676527"/>
+          <a:ext cx="2375306" cy="534762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>If(Comp1)</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1000"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Add EM1 requirement</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1000"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>readTemperatureSi7021()</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2369820</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>161539</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2245766</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>124801</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="TextBox 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE8F348C-9B6D-46B8-B74C-A9097540BD93}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4160520" y="14974819"/>
+          <a:ext cx="2375306" cy="534762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>If(I2C Complete)</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1000"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Remove EM1 requirement</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1000"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>reportTemperatureSi7021()</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1524,10 +3388,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B23" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="15.45" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1983,14 +3847,26 @@
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
     </row>
+    <row r="40" spans="1:6" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A40:F40"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>